<commit_message>
update `led-bar-pcb` BOM to fix resistors values update `caravel-Nucleo-v2-M.2` BOM to remove flexy pins from the previous iteration
</commit_message>
<xml_diff>
--- a/hardware/caravel-Nucleo-v2-M.2/caravel-Nucleo-v2-M.2.xlsx
+++ b/hardware/caravel-Nucleo-v2-M.2/caravel-Nucleo-v2-M.2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t xml:space="preserve">Designators</t>
   </si>
@@ -296,12 +296,6 @@
   </si>
   <si>
     <t xml:space="preserve">NOTE - install on backside of PCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FlexyPins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">see link</t>
   </si>
 </sst>
 </file>
@@ -550,10 +544,10 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.66796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.67578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.33"/>
@@ -1128,21 +1122,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>93</v>
-      </c>
+      <c r="D35" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1178,7 +1158,6 @@
     <hyperlink ref="D32" r:id="rId30" display="SKQGADE010"/>
     <hyperlink ref="D33" r:id="rId31" display="77311-118-03LF"/>
     <hyperlink ref="D34" r:id="rId32" display="SSQ-126-23-G-D"/>
-    <hyperlink ref="D35" r:id="rId33" display="FlexyPins"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>